<commit_message>
update on journal and db design
fix on datanomorakundetail
added new table daily_journal (change in db design)
change on visual form transasksi journalharian
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v2.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v2.beta.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="310">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -954,7 +954,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -969,19 +969,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -1022,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1030,11 +1030,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1342,10 +1343,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q335"/>
+  <dimension ref="B1:Q336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
-      <selection activeCell="E291" sqref="E291"/>
+    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
+      <selection activeCell="D300" sqref="D300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4682,178 +4683,178 @@
     </row>
     <row r="262" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B262" s="1"/>
-      <c r="C262" s="5" t="s">
+      <c r="C262" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D262" s="5" t="s">
+      <c r="D262" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E262" s="5" t="s">
+      <c r="E262" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F262" s="5" t="s">
+      <c r="F262" s="6" t="s">
         <v>215</v>
       </c>
       <c r="G262" s="1"/>
     </row>
     <row r="263" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B263" s="1"/>
-      <c r="C263" s="5"/>
-      <c r="D263" s="5" t="s">
+      <c r="C263" s="6"/>
+      <c r="D263" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E263" s="5" t="s">
+      <c r="E263" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F263" s="5" t="s">
+      <c r="F263" s="6" t="s">
         <v>215</v>
       </c>
       <c r="G263" s="1"/>
     </row>
     <row r="264" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B264" s="1"/>
-      <c r="C264" s="5"/>
-      <c r="D264" s="5" t="s">
+      <c r="C264" s="6"/>
+      <c r="D264" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E264" s="5"/>
-      <c r="F264" s="5" t="s">
+      <c r="E264" s="6"/>
+      <c r="F264" s="6" t="s">
         <v>213</v>
       </c>
       <c r="G264" s="1"/>
     </row>
     <row r="265" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B265" s="1"/>
-      <c r="C265" s="5"/>
-      <c r="D265" s="5" t="s">
+      <c r="C265" s="6"/>
+      <c r="D265" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E265" s="5"/>
-      <c r="F265" s="5" t="s">
+      <c r="E265" s="6"/>
+      <c r="F265" s="6" t="s">
         <v>214</v>
       </c>
       <c r="G265" s="1"/>
     </row>
     <row r="266" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B266" s="1"/>
-      <c r="C266" s="5"/>
-      <c r="D266" s="5" t="s">
+      <c r="C266" s="6"/>
+      <c r="D266" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E266" s="5"/>
-      <c r="F266" s="5" t="s">
+      <c r="E266" s="6"/>
+      <c r="F266" s="6" t="s">
         <v>214</v>
       </c>
       <c r="G266" s="1"/>
     </row>
     <row r="267" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B267" s="1"/>
-      <c r="C267" s="5"/>
-      <c r="D267" s="5" t="s">
+      <c r="C267" s="6"/>
+      <c r="D267" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E267" s="5"/>
-      <c r="F267" s="5" t="s">
+      <c r="E267" s="6"/>
+      <c r="F267" s="6" t="s">
         <v>213</v>
       </c>
       <c r="G267" s="1"/>
     </row>
     <row r="268" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B268" s="1"/>
-      <c r="C268" s="5"/>
-      <c r="D268" s="5" t="s">
+      <c r="C268" s="6"/>
+      <c r="D268" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E268" s="5"/>
-      <c r="F268" s="5" t="s">
+      <c r="E268" s="6"/>
+      <c r="F268" s="6" t="s">
         <v>212</v>
       </c>
       <c r="G268" s="1"/>
     </row>
     <row r="269" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
-      <c r="C269" s="5"/>
-      <c r="D269" s="5" t="s">
+      <c r="C269" s="6"/>
+      <c r="D269" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E269" s="5"/>
-      <c r="F269" s="5" t="s">
+      <c r="E269" s="6"/>
+      <c r="F269" s="6" t="s">
         <v>63</v>
       </c>
       <c r="G269" s="1"/>
     </row>
     <row r="270" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B270" s="1"/>
-      <c r="C270" s="5"/>
-      <c r="D270" s="5" t="s">
+      <c r="C270" s="6"/>
+      <c r="D270" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E270" s="5"/>
-      <c r="F270" s="5" t="s">
+      <c r="E270" s="6"/>
+      <c r="F270" s="6" t="s">
         <v>213</v>
       </c>
       <c r="G270" s="1"/>
     </row>
     <row r="271" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B271" s="1"/>
-      <c r="C271" s="1"/>
-      <c r="D271" s="1"/>
-      <c r="E271" s="1"/>
-      <c r="F271" s="1"/>
+      <c r="C271" s="6"/>
+      <c r="D271" s="6"/>
+      <c r="E271" s="6"/>
+      <c r="F271" s="6"/>
       <c r="G271" s="1"/>
     </row>
     <row r="272" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B272" s="1"/>
-      <c r="C272" s="5" t="s">
+      <c r="C272" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="D272" s="5" t="s">
+      <c r="D272" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E272" s="5" t="s">
+      <c r="E272" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F272" s="5" t="s">
+      <c r="F272" s="6" t="s">
         <v>215</v>
       </c>
       <c r="G272" s="1"/>
     </row>
     <row r="273" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B273" s="1"/>
-      <c r="C273" s="5"/>
-      <c r="D273" s="5" t="s">
+      <c r="C273" s="6"/>
+      <c r="D273" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="E273" s="5" t="s">
+      <c r="E273" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F273" s="5" t="s">
+      <c r="F273" s="6" t="s">
         <v>211</v>
       </c>
       <c r="G273" s="1"/>
     </row>
     <row r="274" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B274" s="1"/>
-      <c r="C274" s="5"/>
-      <c r="D274" s="5" t="s">
+      <c r="C274" s="6"/>
+      <c r="D274" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E274" s="5" t="s">
+      <c r="E274" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F274" s="5" t="s">
+      <c r="F274" s="6" t="s">
         <v>151</v>
       </c>
       <c r="G274" s="1"/>
     </row>
     <row r="275" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B275" s="1"/>
-      <c r="C275" s="5"/>
-      <c r="D275" s="5" t="s">
+      <c r="C275" s="6"/>
+      <c r="D275" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E275" s="5"/>
-      <c r="F275" s="5" t="s">
+      <c r="E275" s="6"/>
+      <c r="F275" s="6" t="s">
         <v>213</v>
       </c>
       <c r="G275" s="1"/>
@@ -4990,56 +4991,56 @@
       <c r="B287" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C287" s="1" t="s">
+      <c r="C287" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D287" s="6" t="s">
+      <c r="D287" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E287" s="6" t="s">
+      <c r="E287" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F287" s="6" t="s">
+      <c r="F287" s="8" t="s">
         <v>211</v>
       </c>
       <c r="G287" s="1"/>
     </row>
     <row r="288" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B288" s="1"/>
-      <c r="C288" s="1"/>
-      <c r="D288" s="6" t="s">
+      <c r="C288" s="8"/>
+      <c r="D288" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E288" s="6" t="s">
+      <c r="E288" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F288" s="6" t="s">
+      <c r="F288" s="8" t="s">
         <v>215</v>
       </c>
       <c r="G288" s="1"/>
     </row>
     <row r="289" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B289" s="1"/>
-      <c r="C289" s="1"/>
-      <c r="D289" s="1" t="s">
+      <c r="C289" s="8"/>
+      <c r="D289" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E289" s="1" t="s">
+      <c r="E289" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F289" s="1" t="s">
+      <c r="F289" s="8" t="s">
         <v>233</v>
       </c>
       <c r="G289" s="1"/>
     </row>
     <row r="290" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B290" s="1"/>
-      <c r="C290" s="1"/>
-      <c r="D290" s="6" t="s">
+      <c r="C290" s="8"/>
+      <c r="D290" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="E290" s="6"/>
-      <c r="F290" s="6" t="s">
+      <c r="E290" s="8"/>
+      <c r="F290" s="8" t="s">
         <v>226</v>
       </c>
       <c r="G290" s="1"/>
@@ -5049,36 +5050,36 @@
     </row>
     <row r="291" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B291" s="1"/>
-      <c r="C291" s="1"/>
-      <c r="D291" s="1" t="s">
+      <c r="C291" s="8"/>
+      <c r="D291" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="E291" s="1"/>
-      <c r="F291" s="1" t="s">
+      <c r="E291" s="8"/>
+      <c r="F291" s="8" t="s">
         <v>226</v>
       </c>
       <c r="G291" s="1"/>
     </row>
     <row r="292" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B292" s="1"/>
-      <c r="C292" s="1"/>
-      <c r="D292" s="1"/>
-      <c r="E292" s="1"/>
-      <c r="F292" s="1"/>
+      <c r="C292" s="8"/>
+      <c r="D292" s="8"/>
+      <c r="E292" s="8"/>
+      <c r="F292" s="8"/>
       <c r="G292" s="1"/>
     </row>
     <row r="293" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B293" s="1"/>
-      <c r="C293" s="6" t="s">
+      <c r="C293" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="D293" s="6" t="s">
+      <c r="D293" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="E293" s="6" t="s">
+      <c r="E293" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F293" s="6" t="s">
+      <c r="F293" s="8" t="s">
         <v>226</v>
       </c>
       <c r="G293" s="1"/>
@@ -5088,14 +5089,14 @@
     </row>
     <row r="294" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B294" s="1"/>
-      <c r="C294" s="6"/>
-      <c r="D294" s="6" t="s">
+      <c r="C294" s="8"/>
+      <c r="D294" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="E294" s="6" t="s">
+      <c r="E294" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F294" s="6" t="s">
+      <c r="F294" s="8" t="s">
         <v>308</v>
       </c>
       <c r="G294" s="1"/>
@@ -5337,38 +5338,36 @@
     <row r="314" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
-      <c r="D314" s="1"/>
-      <c r="E314" s="1"/>
-      <c r="F314" s="1"/>
+      <c r="D314" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E314" s="5"/>
+      <c r="F314" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="G314" s="1"/>
     </row>
     <row r="315" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B315" s="1"/>
-      <c r="C315" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D315" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E315" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F315" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="C315" s="1"/>
+      <c r="D315" s="1"/>
+      <c r="E315" s="1"/>
+      <c r="F315" s="1"/>
       <c r="G315" s="1"/>
     </row>
     <row r="316" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B316" s="1"/>
-      <c r="C316" s="1"/>
+      <c r="C316" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D316" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E316" t="s">
-        <v>278</v>
+        <v>140</v>
+      </c>
+      <c r="E316" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="F316" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G316" s="1"/>
     </row>
@@ -5376,46 +5375,46 @@
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
       <c r="D317" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E317" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="E317" t="s">
+        <v>278</v>
+      </c>
       <c r="F317" s="1" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
       <c r="G317" s="1"/>
     </row>
     <row r="318" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
-      <c r="D318" s="1"/>
+      <c r="D318" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="E318" s="1"/>
-      <c r="F318" s="1"/>
+      <c r="F318" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="G318" s="1"/>
     </row>
     <row r="319" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B319" s="1"/>
-      <c r="C319" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D319" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E319" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F319" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="C319" s="1"/>
+      <c r="D319" s="1"/>
+      <c r="E319" s="1"/>
+      <c r="F319" s="1"/>
       <c r="G319" s="1"/>
     </row>
     <row r="320" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B320" s="1"/>
-      <c r="C320" s="1"/>
+      <c r="C320" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="D320" s="1" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="E320" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F320" s="1" t="s">
         <v>215</v>
@@ -5426,11 +5425,13 @@
       <c r="B321" s="1"/>
       <c r="C321" s="1"/>
       <c r="D321" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E321" s="1"/>
+        <v>275</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F321" s="1" t="s">
-        <v>151</v>
+        <v>215</v>
       </c>
       <c r="G321" s="1"/>
     </row>
@@ -5438,11 +5439,11 @@
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
       <c r="D322" s="1" t="s">
-        <v>140</v>
+        <v>292</v>
       </c>
       <c r="E322" s="1"/>
       <c r="F322" s="1" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="G322" s="1"/>
     </row>
@@ -5450,11 +5451,11 @@
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
       <c r="D323" s="1" t="s">
-        <v>293</v>
+        <v>140</v>
       </c>
       <c r="E323" s="1"/>
       <c r="F323" s="1" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="G323" s="1"/>
     </row>
@@ -5462,11 +5463,11 @@
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
       <c r="D324" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E324" s="1"/>
       <c r="F324" s="1" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="G324" s="1"/>
     </row>
@@ -5474,46 +5475,44 @@
       <c r="B325" s="1"/>
       <c r="C325" s="1"/>
       <c r="D325" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E325" s="1"/>
       <c r="F325" s="1" t="s">
-        <v>189</v>
+        <v>63</v>
       </c>
       <c r="G325" s="1"/>
     </row>
     <row r="326" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B326" s="1"/>
       <c r="C326" s="1"/>
-      <c r="D326" s="1"/>
+      <c r="D326" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="E326" s="1"/>
-      <c r="F326" s="1"/>
+      <c r="F326" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="G326" s="1"/>
     </row>
     <row r="327" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B327" s="1"/>
-      <c r="C327" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D327" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E327" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F327" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="C327" s="1"/>
+      <c r="D327" s="1"/>
+      <c r="E327" s="1"/>
+      <c r="F327" s="1"/>
       <c r="G327" s="1"/>
     </row>
     <row r="328" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B328" s="1"/>
-      <c r="C328" s="1"/>
+      <c r="C328" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D328" s="1" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="E328" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F328" s="1" t="s">
         <v>215</v>
@@ -5524,11 +5523,13 @@
       <c r="B329" s="1"/>
       <c r="C329" s="1"/>
       <c r="D329" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E329" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="E329" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F329" s="1" t="s">
-        <v>151</v>
+        <v>215</v>
       </c>
       <c r="G329" s="1"/>
     </row>
@@ -5536,11 +5537,11 @@
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
       <c r="D330" s="1" t="s">
-        <v>140</v>
+        <v>292</v>
       </c>
       <c r="E330" s="1"/>
       <c r="F330" s="1" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="G330" s="1"/>
     </row>
@@ -5548,11 +5549,11 @@
       <c r="B331" s="1"/>
       <c r="C331" s="1"/>
       <c r="D331" s="1" t="s">
-        <v>293</v>
+        <v>140</v>
       </c>
       <c r="E331" s="1"/>
       <c r="F331" s="1" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="G331" s="1"/>
     </row>
@@ -5560,11 +5561,11 @@
       <c r="B332" s="1"/>
       <c r="C332" s="1"/>
       <c r="D332" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E332" s="1"/>
       <c r="F332" s="1" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="G332" s="1"/>
     </row>
@@ -5572,16 +5573,28 @@
       <c r="B333" s="1"/>
       <c r="C333" s="1"/>
       <c r="D333" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E333" s="1"/>
       <c r="F333" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G333" s="1"/>
+    </row>
+    <row r="334" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B334" s="1"/>
+      <c r="C334" s="1"/>
+      <c r="D334" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E334" s="1"/>
+      <c r="F334" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G333" s="1"/>
-    </row>
-    <row r="335" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B335" t="s">
+      <c r="G334" s="1"/>
+    </row>
+    <row r="336" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B336" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update table and note of flow
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v2.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v2.beta.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="310">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -1032,10 +1032,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1343,10 +1343,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q336"/>
+  <dimension ref="B1:Q337"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="D300" sqref="D300"/>
+      <selection activeCell="D315" sqref="D315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,7 +2769,7 @@
       <c r="D108" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E108" s="7" t="s">
+      <c r="E108" s="8" t="s">
         <v>172</v>
       </c>
       <c r="F108" s="1" t="s">
@@ -2783,7 +2783,7 @@
       <c r="D109" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E109" s="7"/>
+      <c r="E109" s="8"/>
       <c r="F109" s="1" t="s">
         <v>233</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="D110" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E110" s="7"/>
+      <c r="E110" s="8"/>
       <c r="F110" s="1" t="s">
         <v>233</v>
       </c>
@@ -2807,7 +2807,7 @@
       <c r="D111" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E111" s="7"/>
+      <c r="E111" s="8"/>
       <c r="F111" s="1" t="s">
         <v>233</v>
       </c>
@@ -4991,56 +4991,56 @@
       <c r="B287" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C287" s="8" t="s">
+      <c r="C287" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D287" s="8" t="s">
+      <c r="D287" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E287" s="8" t="s">
+      <c r="E287" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="F287" s="8" t="s">
+      <c r="F287" s="7" t="s">
         <v>211</v>
       </c>
       <c r="G287" s="1"/>
     </row>
     <row r="288" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B288" s="1"/>
-      <c r="C288" s="8"/>
-      <c r="D288" s="8" t="s">
+      <c r="C288" s="7"/>
+      <c r="D288" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E288" s="8" t="s">
+      <c r="E288" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F288" s="8" t="s">
+      <c r="F288" s="7" t="s">
         <v>215</v>
       </c>
       <c r="G288" s="1"/>
     </row>
     <row r="289" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B289" s="1"/>
-      <c r="C289" s="8"/>
-      <c r="D289" s="8" t="s">
+      <c r="C289" s="7"/>
+      <c r="D289" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E289" s="8" t="s">
+      <c r="E289" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F289" s="8" t="s">
+      <c r="F289" s="7" t="s">
         <v>233</v>
       </c>
       <c r="G289" s="1"/>
     </row>
     <row r="290" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B290" s="1"/>
-      <c r="C290" s="8"/>
-      <c r="D290" s="8" t="s">
+      <c r="C290" s="7"/>
+      <c r="D290" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="E290" s="8"/>
-      <c r="F290" s="8" t="s">
+      <c r="E290" s="7"/>
+      <c r="F290" s="7" t="s">
         <v>226</v>
       </c>
       <c r="G290" s="1"/>
@@ -5050,36 +5050,36 @@
     </row>
     <row r="291" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B291" s="1"/>
-      <c r="C291" s="8"/>
-      <c r="D291" s="8" t="s">
+      <c r="C291" s="7"/>
+      <c r="D291" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="E291" s="8"/>
-      <c r="F291" s="8" t="s">
+      <c r="E291" s="7"/>
+      <c r="F291" s="7" t="s">
         <v>226</v>
       </c>
       <c r="G291" s="1"/>
     </row>
     <row r="292" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B292" s="1"/>
-      <c r="C292" s="8"/>
-      <c r="D292" s="8"/>
-      <c r="E292" s="8"/>
-      <c r="F292" s="8"/>
+      <c r="C292" s="7"/>
+      <c r="D292" s="7"/>
+      <c r="E292" s="7"/>
+      <c r="F292" s="7"/>
       <c r="G292" s="1"/>
     </row>
     <row r="293" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B293" s="1"/>
-      <c r="C293" s="8" t="s">
+      <c r="C293" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D293" s="8" t="s">
+      <c r="D293" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="E293" s="8" t="s">
+      <c r="E293" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F293" s="8" t="s">
+      <c r="F293" s="7" t="s">
         <v>226</v>
       </c>
       <c r="G293" s="1"/>
@@ -5089,14 +5089,14 @@
     </row>
     <row r="294" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B294" s="1"/>
-      <c r="C294" s="8"/>
-      <c r="D294" s="8" t="s">
+      <c r="C294" s="7"/>
+      <c r="D294" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="E294" s="8" t="s">
+      <c r="E294" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F294" s="8" t="s">
+      <c r="F294" s="7" t="s">
         <v>308</v>
       </c>
       <c r="G294" s="1"/>
@@ -5339,7 +5339,7 @@
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
       <c r="D314" s="5" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="E314" s="5"/>
       <c r="F314" s="5" t="s">
@@ -5350,38 +5350,36 @@
     <row r="315" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
-      <c r="D315" s="1"/>
-      <c r="E315" s="1"/>
-      <c r="F315" s="1"/>
+      <c r="D315" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E315" s="5"/>
+      <c r="F315" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="G315" s="1"/>
     </row>
     <row r="316" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B316" s="1"/>
-      <c r="C316" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D316" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E316" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F316" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="C316" s="1"/>
+      <c r="D316" s="1"/>
+      <c r="E316" s="1"/>
+      <c r="F316" s="1"/>
       <c r="G316" s="1"/>
     </row>
     <row r="317" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B317" s="1"/>
-      <c r="C317" s="1"/>
+      <c r="C317" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D317" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E317" t="s">
-        <v>278</v>
+        <v>140</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="F317" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G317" s="1"/>
     </row>
@@ -5389,46 +5387,46 @@
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
       <c r="D318" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E318" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="E318" t="s">
+        <v>278</v>
+      </c>
       <c r="F318" s="1" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
       <c r="G318" s="1"/>
     </row>
     <row r="319" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B319" s="1"/>
       <c r="C319" s="1"/>
-      <c r="D319" s="1"/>
+      <c r="D319" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="E319" s="1"/>
-      <c r="F319" s="1"/>
+      <c r="F319" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="G319" s="1"/>
     </row>
     <row r="320" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B320" s="1"/>
-      <c r="C320" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D320" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E320" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F320" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="C320" s="1"/>
+      <c r="D320" s="1"/>
+      <c r="E320" s="1"/>
+      <c r="F320" s="1"/>
       <c r="G320" s="1"/>
     </row>
     <row r="321" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B321" s="1"/>
-      <c r="C321" s="1"/>
+      <c r="C321" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="D321" s="1" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="E321" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F321" s="1" t="s">
         <v>215</v>
@@ -5439,11 +5437,13 @@
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
       <c r="D322" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E322" s="1"/>
+        <v>275</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F322" s="1" t="s">
-        <v>151</v>
+        <v>215</v>
       </c>
       <c r="G322" s="1"/>
     </row>
@@ -5451,11 +5451,11 @@
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
       <c r="D323" s="1" t="s">
-        <v>140</v>
+        <v>292</v>
       </c>
       <c r="E323" s="1"/>
       <c r="F323" s="1" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="G323" s="1"/>
     </row>
@@ -5463,11 +5463,11 @@
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
       <c r="D324" s="1" t="s">
-        <v>293</v>
+        <v>140</v>
       </c>
       <c r="E324" s="1"/>
       <c r="F324" s="1" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="G324" s="1"/>
     </row>
@@ -5475,11 +5475,11 @@
       <c r="B325" s="1"/>
       <c r="C325" s="1"/>
       <c r="D325" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E325" s="1"/>
       <c r="F325" s="1" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="G325" s="1"/>
     </row>
@@ -5487,46 +5487,44 @@
       <c r="B326" s="1"/>
       <c r="C326" s="1"/>
       <c r="D326" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E326" s="1"/>
       <c r="F326" s="1" t="s">
-        <v>189</v>
+        <v>63</v>
       </c>
       <c r="G326" s="1"/>
     </row>
     <row r="327" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B327" s="1"/>
       <c r="C327" s="1"/>
-      <c r="D327" s="1"/>
+      <c r="D327" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="E327" s="1"/>
-      <c r="F327" s="1"/>
+      <c r="F327" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="G327" s="1"/>
     </row>
     <row r="328" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B328" s="1"/>
-      <c r="C328" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D328" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E328" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F328" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="C328" s="1"/>
+      <c r="D328" s="1"/>
+      <c r="E328" s="1"/>
+      <c r="F328" s="1"/>
       <c r="G328" s="1"/>
     </row>
     <row r="329" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B329" s="1"/>
-      <c r="C329" s="1"/>
+      <c r="C329" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D329" s="1" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="E329" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F329" s="1" t="s">
         <v>215</v>
@@ -5537,11 +5535,13 @@
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
       <c r="D330" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E330" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F330" s="1" t="s">
-        <v>151</v>
+        <v>215</v>
       </c>
       <c r="G330" s="1"/>
     </row>
@@ -5549,11 +5549,11 @@
       <c r="B331" s="1"/>
       <c r="C331" s="1"/>
       <c r="D331" s="1" t="s">
-        <v>140</v>
+        <v>292</v>
       </c>
       <c r="E331" s="1"/>
       <c r="F331" s="1" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="G331" s="1"/>
     </row>
@@ -5561,11 +5561,11 @@
       <c r="B332" s="1"/>
       <c r="C332" s="1"/>
       <c r="D332" s="1" t="s">
-        <v>293</v>
+        <v>140</v>
       </c>
       <c r="E332" s="1"/>
       <c r="F332" s="1" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="G332" s="1"/>
     </row>
@@ -5573,11 +5573,11 @@
       <c r="B333" s="1"/>
       <c r="C333" s="1"/>
       <c r="D333" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E333" s="1"/>
       <c r="F333" s="1" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="G333" s="1"/>
     </row>
@@ -5585,16 +5585,28 @@
       <c r="B334" s="1"/>
       <c r="C334" s="1"/>
       <c r="D334" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E334" s="1"/>
       <c r="F334" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G334" s="1"/>
+    </row>
+    <row r="335" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B335" s="1"/>
+      <c r="C335" s="1"/>
+      <c r="D335" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E335" s="1"/>
+      <c r="F335" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G334" s="1"/>
-    </row>
-    <row r="336" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B336" t="s">
+      <c r="G335" s="1"/>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B337" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>